<commit_message>
zmieniona struktura zwracanych synsetow i ich rankingu
</commit_message>
<xml_diff>
--- a/ontologie.xlsx
+++ b/ontologie.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinez/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinez/Projects/wordnet-attributes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405B3A17-88B6-194B-A73B-4D7A8510DF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2B70A6-7A96-2148-9A43-ECAAAAC6ADA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="3600" windowWidth="27640" windowHeight="16860" activeTab="3" xr2:uid="{10C6D98F-35D3-6D49-81BC-D85E11FE798E}"/>
   </bookViews>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
   <si>
     <t>Concept</t>
   </si>
@@ -210,9 +209,6 @@
     <t>hasSubmisssionInstruction: string</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
     <t>City_of_conference: string</t>
   </si>
   <si>
@@ -325,6 +321,15 @@
   </si>
   <si>
     <t>Organization</t>
+  </si>
+  <si>
+    <t>tokenized definition</t>
+  </si>
+  <si>
+    <t>calculated similarity</t>
+  </si>
+  <si>
+    <t>definition</t>
   </si>
 </sst>
 </file>
@@ -677,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D014666-825E-8B4E-A4A9-E4A275E66E24}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +694,7 @@
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,8 +704,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -708,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -716,7 +730,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -724,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -732,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -740,7 +754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -748,7 +762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -756,7 +770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -764,7 +778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -772,7 +786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -780,7 +794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -788,7 +802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -796,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -804,7 +818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -812,7 +826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -883,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE795582-1486-2D47-96BB-D7325349B572}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,7 +909,7 @@
     <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,8 +919,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -914,7 +937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -922,7 +945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -930,7 +953,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -938,7 +961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -946,7 +969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -954,7 +977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -962,7 +985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -970,7 +993,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -978,7 +1001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -986,7 +1009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -994,7 +1017,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1002,7 +1025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1010,7 +1033,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1018,7 +1041,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1081,133 +1104,149 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314FBD93-D461-7848-9ADA-329F23EF5524}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1107EA83-E341-0049-A7C9-CF097FC2102E}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,181 +1256,190 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
         <v>89</v>
-      </c>
-      <c r="B22" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1407,7 +1455,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1423,7 +1471,7 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1455,12 +1503,12 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
         <v>46</v>
@@ -1468,7 +1516,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
         <v>53</v>
@@ -1476,5 +1524,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>